<commit_message>
folder skoonmaak. file voordat geshare. voledige file
</commit_message>
<xml_diff>
--- a/plots/author keyword table.xlsx
+++ b/plots/author keyword table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13950" windowHeight="4335"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="13950" windowHeight="4335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,23 +74,23 @@
     <t>oilseed rape</t>
   </si>
   <si>
-    <t>fungi</t>
-  </si>
-  <si>
-    <t>antifungal</t>
+    <t>sunflower</t>
+  </si>
+  <si>
+    <t>sclerotinia stem rot</t>
+  </si>
+  <si>
+    <t>sclerotinia</t>
   </si>
   <si>
     <t>disease resistance</t>
-  </si>
-  <si>
-    <t>mycoparasitism</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +102,11 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lucida Sans"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -125,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -133,6 +138,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,207 +422,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B20"/>
+      <selection activeCell="B20" sqref="A1:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>867</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3">
-        <v>70</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3">
-        <v>49</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3">
-        <v>47</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="3">
-        <v>38</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
-        <v>37</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3">
-        <v>31</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="B11" s="3">
-        <v>28</v>
-      </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="3">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="B13" s="3">
-        <v>24</v>
-      </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
-        <v>22</v>
-      </c>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B16" s="3">
+        <v>62</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="3">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="B17" s="3">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2">
+        <v>59</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="3">
-        <v>16</v>
-      </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="B19" s="3">
+        <v>53</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="3">
-        <v>16</v>
-      </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="2">
-        <v>16</v>
-      </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="B20" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="A1:B20">
+    <sortCondition descending="1" ref="B1:B20"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>